<commit_message>
[~] Alternated tests to exclude ipv4-addressing, as this skill was already practically maxed out for all participants [+] Added a standard deviation test to determine the differences between the knowledge of skills. Calculating the standard deviation for two points within a data set is however somewhat questionable.
</commit_message>
<xml_diff>
--- a/data/pre_evaluation.xlsx
+++ b/data/pre_evaluation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soennecken\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8300E2E-C8C9-40C7-96E9-89A102CD4EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C25E71D-9121-4A47-BACF-D5B3FA33C88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pretest" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="mappings" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pretest!$A$1:$E$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pretest!$A$1:$C$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">posttest!$A$1:$C$53</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>User</t>
   </si>
@@ -52,12 +53,6 @@
   </si>
   <si>
     <t>Correct</t>
-  </si>
-  <si>
-    <t>Incorrect</t>
-  </si>
-  <si>
-    <t>Unnecessary</t>
   </si>
   <si>
     <t>Test</t>
@@ -160,7 +155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,7 +204,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -487,18 +482,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -508,14 +500,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -525,14 +511,8 @@
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -542,14 +522,8 @@
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -559,14 +533,8 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -576,14 +544,8 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -593,14 +555,8 @@
       <c r="C6">
         <v>10</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -610,14 +566,8 @@
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -627,14 +577,8 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -644,14 +588,8 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="2">
         <v>3</v>
       </c>
@@ -661,14 +599,8 @@
       <c r="C10">
         <v>5</v>
       </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -678,14 +610,8 @@
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11">
-        <v>5</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -695,14 +621,8 @@
       <c r="C12">
         <v>0</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -710,16 +630,10 @@
         <v>4</v>
       </c>
       <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="2">
         <v>4</v>
       </c>
@@ -729,14 +643,8 @@
       <c r="C14">
         <v>4</v>
       </c>
-      <c r="D14">
-        <v>6</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="2">
         <v>4</v>
       </c>
@@ -746,14 +654,8 @@
       <c r="C15">
         <v>0</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="2">
         <v>4</v>
       </c>
@@ -763,14 +665,8 @@
       <c r="C16">
         <v>0</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -780,14 +676,8 @@
       <c r="C17">
         <v>0</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="2">
         <v>5</v>
       </c>
@@ -797,14 +687,8 @@
       <c r="C18">
         <v>0</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="2">
         <v>5</v>
       </c>
@@ -814,14 +698,8 @@
       <c r="C19">
         <v>0</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="2">
         <v>5</v>
       </c>
@@ -831,14 +709,8 @@
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="2">
         <v>5</v>
       </c>
@@ -848,14 +720,8 @@
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="2">
         <v>6</v>
       </c>
@@ -865,14 +731,8 @@
       <c r="C22">
         <v>0</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="2">
         <v>6</v>
       </c>
@@ -882,14 +742,8 @@
       <c r="C23">
         <v>3</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="2">
         <v>6</v>
       </c>
@@ -899,14 +753,8 @@
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="2">
         <v>6</v>
       </c>
@@ -916,14 +764,8 @@
       <c r="C25">
         <v>0</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="2">
         <v>7</v>
       </c>
@@ -933,14 +775,8 @@
       <c r="C26">
         <v>6</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="2">
         <v>7</v>
       </c>
@@ -950,14 +786,8 @@
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="D27">
-        <v>3</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="2">
         <v>7</v>
       </c>
@@ -967,14 +797,8 @@
       <c r="C28">
         <v>0</v>
       </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="2">
         <v>7</v>
       </c>
@@ -984,14 +808,8 @@
       <c r="C29">
         <v>0</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="2">
         <v>8</v>
       </c>
@@ -1001,14 +819,8 @@
       <c r="C30">
         <v>3</v>
       </c>
-      <c r="D30">
-        <v>3</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="2">
         <v>8</v>
       </c>
@@ -1018,14 +830,8 @@
       <c r="C31">
         <v>0</v>
       </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="2">
         <v>8</v>
       </c>
@@ -1035,14 +841,8 @@
       <c r="C32">
         <v>0</v>
       </c>
-      <c r="D32">
-        <v>2</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="2">
         <v>8</v>
       </c>
@@ -1052,14 +852,8 @@
       <c r="C33">
         <v>0</v>
       </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="2">
         <v>9</v>
       </c>
@@ -1069,14 +863,8 @@
       <c r="C34">
         <v>4</v>
       </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="2">
         <v>9</v>
       </c>
@@ -1086,14 +874,8 @@
       <c r="C35">
         <v>2</v>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="2">
         <v>9</v>
       </c>
@@ -1103,14 +885,8 @@
       <c r="C36">
         <v>0</v>
       </c>
-      <c r="D36">
-        <v>2</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="2">
         <v>9</v>
       </c>
@@ -1120,14 +896,8 @@
       <c r="C37">
         <v>0</v>
       </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="2">
         <v>10</v>
       </c>
@@ -1137,14 +907,8 @@
       <c r="C38">
         <v>10</v>
       </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="2">
         <v>10</v>
       </c>
@@ -1154,14 +918,8 @@
       <c r="C39">
         <v>2</v>
       </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="2">
         <v>10</v>
       </c>
@@ -1169,16 +927,10 @@
         <v>3</v>
       </c>
       <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="2">
         <v>10</v>
       </c>
@@ -1188,14 +940,8 @@
       <c r="C41">
         <v>2</v>
       </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="2">
         <v>11</v>
       </c>
@@ -1205,14 +951,8 @@
       <c r="C42">
         <v>0</v>
       </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="2">
         <v>11</v>
       </c>
@@ -1222,14 +962,8 @@
       <c r="C43">
         <v>0</v>
       </c>
-      <c r="D43">
-        <v>2</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" s="2">
         <v>11</v>
       </c>
@@ -1237,16 +971,10 @@
         <v>3</v>
       </c>
       <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="2">
         <v>11</v>
       </c>
@@ -1256,14 +984,8 @@
       <c r="C45">
         <v>0</v>
       </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="2">
         <v>12</v>
       </c>
@@ -1273,14 +995,8 @@
       <c r="C46">
         <v>4</v>
       </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="2">
         <v>12</v>
       </c>
@@ -1290,14 +1006,8 @@
       <c r="C47">
         <v>0</v>
       </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="2">
         <v>12</v>
       </c>
@@ -1307,14 +1017,8 @@
       <c r="C48">
         <v>0</v>
       </c>
-      <c r="D48">
-        <v>2</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" s="2">
         <v>12</v>
       </c>
@@ -1324,14 +1028,8 @@
       <c r="C49">
         <v>0</v>
       </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" s="2">
         <v>13</v>
       </c>
@@ -1341,14 +1039,8 @@
       <c r="C50">
         <v>4</v>
       </c>
-      <c r="D50">
-        <v>4</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" s="2">
         <v>13</v>
       </c>
@@ -1358,14 +1050,8 @@
       <c r="C51">
         <v>2</v>
       </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" s="2">
         <v>13</v>
       </c>
@@ -1375,14 +1061,8 @@
       <c r="C52">
         <v>0</v>
       </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" s="2">
         <v>13</v>
       </c>
@@ -1392,30 +1072,24 @@
       <c r="C53">
         <v>0</v>
       </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E53" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C53" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1AC0FE7-6080-4F6F-966D-C38A541AD805}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1425,14 +1099,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1442,14 +1110,8 @@
       <c r="C2">
         <v>3</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1459,14 +1121,8 @@
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1476,14 +1132,8 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1493,14 +1143,8 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1510,14 +1154,8 @@
       <c r="C6">
         <v>10</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1527,14 +1165,8 @@
       <c r="C7">
         <v>3</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -1544,14 +1176,8 @@
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -1561,14 +1187,8 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="2">
         <v>3</v>
       </c>
@@ -1578,14 +1198,8 @@
       <c r="C10">
         <v>8</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -1595,14 +1209,8 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -1612,14 +1220,8 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -1629,14 +1231,8 @@
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="2">
         <v>4</v>
       </c>
@@ -1646,14 +1242,8 @@
       <c r="C14">
         <v>6</v>
       </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="2">
         <v>4</v>
       </c>
@@ -1663,14 +1253,8 @@
       <c r="C15">
         <v>2</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="2">
         <v>4</v>
       </c>
@@ -1680,14 +1264,8 @@
       <c r="C16">
         <v>0</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -1697,14 +1275,8 @@
       <c r="C17">
         <v>0</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="2">
         <v>5</v>
       </c>
@@ -1714,14 +1286,8 @@
       <c r="C18">
         <v>0</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="2">
         <v>5</v>
       </c>
@@ -1729,16 +1295,10 @@
         <v>2</v>
       </c>
       <c r="C19">
-        <v>3</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="2">
         <v>5</v>
       </c>
@@ -1748,14 +1308,8 @@
       <c r="C20">
         <v>0</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="2">
         <v>5</v>
       </c>
@@ -1765,14 +1319,8 @@
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="2">
         <v>6</v>
       </c>
@@ -1782,14 +1330,8 @@
       <c r="C22">
         <v>10</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="2">
         <v>6</v>
       </c>
@@ -1799,14 +1341,8 @@
       <c r="C23">
         <v>0</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="2">
         <v>6</v>
       </c>
@@ -1814,16 +1350,10 @@
         <v>3</v>
       </c>
       <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="2">
         <v>6</v>
       </c>
@@ -1833,14 +1363,8 @@
       <c r="C25">
         <v>0</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="2">
         <v>7</v>
       </c>
@@ -1850,14 +1374,8 @@
       <c r="C26">
         <v>3</v>
       </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="2">
         <v>7</v>
       </c>
@@ -1867,14 +1385,8 @@
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="2">
         <v>7</v>
       </c>
@@ -1884,14 +1396,8 @@
       <c r="C28">
         <v>0</v>
       </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="2">
         <v>7</v>
       </c>
@@ -1899,16 +1405,10 @@
         <v>4</v>
       </c>
       <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="2">
         <v>8</v>
       </c>
@@ -1918,14 +1418,8 @@
       <c r="C30">
         <v>5</v>
       </c>
-      <c r="D30">
-        <v>3</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="2">
         <v>8</v>
       </c>
@@ -1935,14 +1429,8 @@
       <c r="C31">
         <v>0</v>
       </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="2">
         <v>8</v>
       </c>
@@ -1952,14 +1440,8 @@
       <c r="C32">
         <v>2</v>
       </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="2">
         <v>8</v>
       </c>
@@ -1969,14 +1451,8 @@
       <c r="C33">
         <v>0</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="2">
         <v>9</v>
       </c>
@@ -1986,14 +1462,8 @@
       <c r="C34">
         <v>6</v>
       </c>
-      <c r="D34">
-        <v>4</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="2">
         <v>9</v>
       </c>
@@ -2003,14 +1473,8 @@
       <c r="C35">
         <v>3</v>
       </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="2">
         <v>9</v>
       </c>
@@ -2020,14 +1484,8 @@
       <c r="C36">
         <v>1</v>
       </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="2">
         <v>9</v>
       </c>
@@ -2037,14 +1495,8 @@
       <c r="C37">
         <v>2</v>
       </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="2">
         <v>10</v>
       </c>
@@ -2054,14 +1506,8 @@
       <c r="C38">
         <v>10</v>
       </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="2">
         <v>10</v>
       </c>
@@ -2071,14 +1517,8 @@
       <c r="C39">
         <v>2</v>
       </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="2">
         <v>10</v>
       </c>
@@ -2088,14 +1528,8 @@
       <c r="C40">
         <v>0</v>
       </c>
-      <c r="D40">
-        <v>2</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="2">
         <v>10</v>
       </c>
@@ -2105,14 +1539,8 @@
       <c r="C41">
         <v>2</v>
       </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="2">
         <v>11</v>
       </c>
@@ -2122,14 +1550,8 @@
       <c r="C42">
         <v>5</v>
       </c>
-      <c r="D42">
-        <v>3</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="2">
         <v>11</v>
       </c>
@@ -2139,14 +1561,8 @@
       <c r="C43">
         <v>0</v>
       </c>
-      <c r="D43">
-        <v>2</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" s="2">
         <v>11</v>
       </c>
@@ -2154,16 +1570,10 @@
         <v>3</v>
       </c>
       <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="2">
         <v>11</v>
       </c>
@@ -2173,14 +1583,8 @@
       <c r="C45">
         <v>0</v>
       </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="2">
         <v>12</v>
       </c>
@@ -2190,14 +1594,8 @@
       <c r="C46">
         <v>5</v>
       </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="2">
         <v>12</v>
       </c>
@@ -2207,14 +1605,8 @@
       <c r="C47">
         <v>0</v>
       </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="2">
         <v>12</v>
       </c>
@@ -2224,14 +1616,8 @@
       <c r="C48">
         <v>2</v>
       </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" s="2">
         <v>12</v>
       </c>
@@ -2241,14 +1627,8 @@
       <c r="C49">
         <v>0</v>
       </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" s="2">
         <v>13</v>
       </c>
@@ -2258,14 +1638,8 @@
       <c r="C50">
         <v>10</v>
       </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" s="2">
         <v>13</v>
       </c>
@@ -2275,14 +1649,8 @@
       <c r="C51">
         <v>3</v>
       </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="E51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" s="2">
         <v>13</v>
       </c>
@@ -2292,14 +1660,8 @@
       <c r="C52">
         <v>0</v>
       </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" s="2">
         <v>13</v>
       </c>
@@ -2309,14 +1671,9 @@
       <c r="C53">
         <v>2</v>
       </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C53" xr:uid="{E1AC0FE7-6080-4F6F-966D-C38A541AD805}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2326,23 +1683,23 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2353,7 +1710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -2364,7 +1721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -2375,7 +1732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -2386,7 +1743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -2397,7 +1754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -2408,7 +1765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -2419,7 +1776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -2443,64 +1800,64 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2508,10 +1865,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2519,10 +1876,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2530,10 +1887,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2541,10 +1898,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2552,10 +1909,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2563,10 +1920,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2574,10 +1931,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2585,10 +1942,10 @@
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2596,54 +1953,54 @@
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2">
+        <v>2</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2">
-        <v>2</v>
-      </c>
-      <c r="C15" s="4" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="2">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>2</v>
-      </c>
-      <c r="B16" s="2">
-        <v>2</v>
-      </c>
-      <c r="C16" s="4" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" s="2">
+        <v>4</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>3</v>
-      </c>
-      <c r="B17" s="2">
-        <v>2</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>4</v>
-      </c>
-      <c r="B18" s="2">
-        <v>2</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="2">
         <v>5</v>
       </c>
@@ -2651,10 +2008,10 @@
         <v>2</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="2">
         <v>6</v>
       </c>
@@ -2662,10 +2019,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="2">
         <v>7</v>
       </c>
@@ -2673,10 +2030,10 @@
         <v>2</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="2">
         <v>8</v>
       </c>
@@ -2684,10 +2041,10 @@
         <v>2</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="2">
         <v>9</v>
       </c>
@@ -2695,10 +2052,10 @@
         <v>2</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="2">
         <v>10</v>
       </c>
@@ -2706,10 +2063,10 @@
         <v>2</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="2">
         <v>11</v>
       </c>
@@ -2717,10 +2074,10 @@
         <v>2</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="2">
         <v>12</v>
       </c>
@@ -2728,10 +2085,10 @@
         <v>2</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="2">
         <v>13</v>
       </c>
@@ -2739,7 +2096,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2751,125 +2108,125 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{970D1068-889D-403B-B5ED-79FDC5518E97}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>